<commit_message>
feat:scraping odds betano, comparando com fairline
</commit_message>
<xml_diff>
--- a/fairlines2023-04-20.xlsx
+++ b/fairlines2023-04-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98987e24a2b0f31d/Área de Trabalho/corner_stats/corner_stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_9681DF0CC6A8C77B17A52B3A30B0E930240123E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4789249-F565-4436-BCCA-DC9381FCD1CC}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_9681DF0CC6A8C77B17A52B3A30B0E930240123E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{222A82F1-1A1D-4597-97A1-9499F9DFEB8C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17880" yWindow="1260" windowWidth="14400" windowHeight="10755" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fairlines" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Odd</t>
+  </si>
+  <si>
+    <t>Resultado</t>
   </si>
 </sst>
 </file>
@@ -188,7 +191,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -226,16 +229,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -253,6 +270,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,11 +563,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -2183,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2922,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,7 +2958,7 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -2949,8 +2971,11 @@
       <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2963,8 +2988,11 @@
       <c r="D2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2977,8 +3005,11 @@
       <c r="D3">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2991,8 +3022,11 @@
       <c r="D4">
         <v>2.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -3005,8 +3039,11 @@
       <c r="D5">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3019,8 +3056,11 @@
       <c r="D6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3033,8 +3073,11 @@
       <c r="D7">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3046,6 +3089,9 @@
       </c>
       <c r="D8">
         <v>1.93</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: xls com oportunidades consolidada + analises
</commit_message>
<xml_diff>
--- a/fairlines2023-04-20.xlsx
+++ b/fairlines2023-04-20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98987e24a2b0f31d/Área de Trabalho/corner_stats/corner_stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_9681DF0CC6A8C77B17A52B3A30B0E930240123E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{222A82F1-1A1D-4597-97A1-9499F9DFEB8C}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_9681DF0CC6A8C77B17A52B3A30B0E930240123E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7E1EC70-D4C1-4FD5-B441-9A93733EA24F}"/>
   <bookViews>
-    <workbookView xWindow="-17880" yWindow="1260" windowWidth="14400" windowHeight="10755" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-1215" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fairlines" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="Fair - Betano" sheetId="3" r:id="rId3"/>
     <sheet name="Oportunidades" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -155,13 +168,16 @@
   </si>
   <si>
     <t>Resultado</t>
+  </si>
+  <si>
+    <t>Probabilidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +197,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -241,10 +272,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -255,9 +287,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2944,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,9 +2991,10 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -2972,10 +3008,13 @@
         <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -2988,11 +3027,15 @@
       <c r="D2">
         <v>2.75</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4">
+        <f>1/(D2+C2)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -3005,11 +3048,15 @@
       <c r="D3">
         <v>2.8</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4">
+        <f>1/(D3+C3)</f>
+        <v>0.42918454935622319</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -3022,11 +3069,15 @@
       <c r="D4">
         <v>2.65</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="4">
+        <f>1/(D4+C4)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -3039,11 +3090,15 @@
       <c r="D5">
         <v>3.6</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="4">
+        <f>1/(D5+C5)</f>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3056,11 +3111,15 @@
       <c r="D6">
         <v>1.3</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="4">
+        <f>1/(D6+C6)</f>
+        <v>0.9009009009009008</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3073,11 +3132,16 @@
       <c r="D7">
         <v>1.57</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <f>1/(D7+C7)</f>
+        <v>0.7246376811594204</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -3090,11 +3154,16 @@
       <c r="D8">
         <v>1.93</v>
       </c>
-      <c r="E8">
-        <v>0</v>
+      <c r="E8" s="4">
+        <f>1/(D8+C8)</f>
+        <v>0.5988023952095809</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>